<commit_message>
Q3 Update - 2025
</commit_message>
<xml_diff>
--- a/Excel-XLSX/UN-AFG.xlsx
+++ b/Excel-XLSX/UN-AFG.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="322">
   <si>
     <t>﻿"page"</t>
   </si>
@@ -87,7 +87,7 @@
     <t>1</t>
   </si>
   <si>
-    <t>rmCC7r</t>
+    <t>MGuy8C</t>
   </si>
   <si>
     <t>1990</t>
@@ -951,16 +951,16 @@
     <t>2024</t>
   </si>
   <si>
-    <t>3221286</t>
-  </si>
-  <si>
-    <t>1111</t>
-  </si>
-  <si>
-    <t>72883</t>
-  </si>
-  <si>
-    <t>1738747</t>
+    <t>3199710</t>
+  </si>
+  <si>
+    <t>22687</t>
+  </si>
+  <si>
+    <t>72886</t>
+  </si>
+  <si>
+    <t>600000</t>
   </si>
   <si>
     <t>123</t>
@@ -972,13 +972,16 @@
     <t>125</t>
   </si>
   <si>
-    <t>34795</t>
-  </si>
-  <si>
-    <t>224</t>
-  </si>
-  <si>
     <t>126</t>
+  </si>
+  <si>
+    <t>20827</t>
+  </si>
+  <si>
+    <t>299</t>
+  </si>
+  <si>
+    <t>127</t>
   </si>
 </sst>
 </file>
@@ -1363,7 +1366,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:V127"/>
+  <dimension ref="A1:V128"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
@@ -9820,16 +9823,16 @@
         <v>310</v>
       </c>
       <c r="F125" s="2" t="s">
-        <v>49</v>
+        <v>107</v>
       </c>
       <c r="G125" s="1" t="s">
-        <v>50</v>
+        <v>108</v>
       </c>
       <c r="H125" s="1" t="s">
-        <v>51</v>
+        <v>109</v>
       </c>
       <c r="I125" s="1" t="s">
-        <v>51</v>
+        <v>109</v>
       </c>
       <c r="J125" s="2" t="s">
         <v>29</v>
@@ -9844,10 +9847,10 @@
         <v>31</v>
       </c>
       <c r="N125" s="2" t="s">
-        <v>132</v>
+        <v>33</v>
       </c>
       <c r="O125" s="2" t="s">
-        <v>145</v>
+        <v>45</v>
       </c>
       <c r="P125" s="2" t="s">
         <v>33</v>
@@ -9888,16 +9891,16 @@
         <v>310</v>
       </c>
       <c r="F126" s="2" t="s">
-        <v>146</v>
+        <v>49</v>
       </c>
       <c r="G126" s="1" t="s">
-        <v>147</v>
+        <v>50</v>
       </c>
       <c r="H126" s="1" t="s">
-        <v>148</v>
+        <v>51</v>
       </c>
       <c r="I126" s="1" t="s">
-        <v>148</v>
+        <v>51</v>
       </c>
       <c r="J126" s="2" t="s">
         <v>29</v>
@@ -9912,10 +9915,10 @@
         <v>31</v>
       </c>
       <c r="N126" s="2" t="s">
-        <v>318</v>
+        <v>132</v>
       </c>
       <c r="O126" s="2" t="s">
-        <v>319</v>
+        <v>165</v>
       </c>
       <c r="P126" s="2" t="s">
         <v>33</v>
@@ -9950,60 +9953,128 @@
         <v>22</v>
       </c>
       <c r="D127" s="2" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="E127" s="2" t="s">
         <v>310</v>
       </c>
       <c r="F127" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="G127" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="H127" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="I127" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="J127" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K127" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L127" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M127" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N127" s="2" t="s">
+        <v>319</v>
+      </c>
+      <c r="O127" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="P127" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q127" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="R127" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="S127" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="T127" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="U127" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="V127" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B128" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D128" s="2" t="s">
+        <v>321</v>
+      </c>
+      <c r="E128" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="F128" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="G127" s="1" t="s">
+      <c r="G128" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H127" s="1" t="s">
+      <c r="H128" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="I127" s="1" t="s">
+      <c r="I128" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="J127" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="K127" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="L127" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="M127" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="N127" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="O127" s="2" t="s">
+      <c r="J128" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K128" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="L128" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M128" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="N128" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="O128" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="P127" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q127" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="R127" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="S127" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="T127" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="U127" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="V127" s="2" t="s">
+      <c r="P128" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q128" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="R128" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="S128" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="T128" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="U128" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="V128" s="2" t="s">
         <v>33</v>
       </c>
     </row>

</xml_diff>